<commit_message>
Merge schema changes to UT IAC London list from PUB-2835
</commit_message>
<xml_diff>
--- a/src/integrationTest/resources/data/non-strategic/ut-iac-judicial-review-london-daily-hearing-list/utIacJudicialReviewLondonDailyHearingList.xlsx
+++ b/src/integrationTest/resources/data/non-strategic/ut-iac-judicial-review-london-daily-hearing-list/utIacJudicialReviewLondonDailyHearingList.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11207"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10311"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kian.kwa/IdeaProjects/pip-data-management/src/integrationTest/resources/data/non-strategic/ut-iac-judicial-review-daily-hearing-list/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/natasha.alker/Repos/pip/pip-data-management/src/integrationTest/resources/data/non-strategic/ut-iac-judicial-review-london-daily-hearing-list/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B2C3DF6-78EB-C04D-B4CC-26EA9474111F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{453A6598-42DF-C248-A67C-6A2832CF4106}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="51900" yWindow="1980" windowWidth="35140" windowHeight="26960" xr2:uid="{0C1F814A-B1E5-C24D-AA62-DAE35072E02F}"/>
+    <workbookView xWindow="460" yWindow="880" windowWidth="35140" windowHeight="19520" xr2:uid="{0C1F814A-B1E5-C24D-AA62-DAE35072E02F}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -65,24 +65,15 @@
     <t>Additional information</t>
   </si>
   <si>
-    <t>Applicant</t>
-  </si>
-  <si>
     <t>representative</t>
   </si>
   <si>
     <t>Location</t>
   </si>
   <si>
-    <t>Applicant A</t>
-  </si>
-  <si>
     <t>Rep A</t>
   </si>
   <si>
-    <t>Applicant B</t>
-  </si>
-  <si>
     <t>Rep B</t>
   </si>
   <si>
@@ -96,6 +87,15 @@
   </si>
   <si>
     <t>Hearing type</t>
+  </si>
+  <si>
+    <t>Case A</t>
+  </si>
+  <si>
+    <t>Case B</t>
+  </si>
+  <si>
+    <t>Case title</t>
   </si>
 </sst>
 </file>
@@ -470,7 +470,7 @@
   <dimension ref="A1:H3"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F1" sqref="F1"/>
+      <selection activeCell="G11" sqref="G11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -485,13 +485,13 @@
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="B1" t="s">
+        <v>19</v>
+      </c>
+      <c r="C1" t="s">
         <v>9</v>
-      </c>
-      <c r="C1" t="s">
-        <v>10</v>
       </c>
       <c r="D1" t="s">
         <v>1</v>
@@ -500,10 +500,10 @@
         <v>7</v>
       </c>
       <c r="F1" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="G1" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="H1" t="s">
         <v>8</v>
@@ -514,10 +514,10 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>12</v>
+        <v>17</v>
       </c>
       <c r="C2" t="s">
-        <v>13</v>
+        <v>11</v>
       </c>
       <c r="D2">
         <v>1234</v>
@@ -526,7 +526,7 @@
         <v>2</v>
       </c>
       <c r="F2" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="G2" t="s">
         <v>4</v>
@@ -537,13 +537,13 @@
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
+        <v>15</v>
+      </c>
+      <c r="B3" t="s">
         <v>18</v>
       </c>
-      <c r="B3" t="s">
-        <v>14</v>
-      </c>
       <c r="C3" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="D3">
         <v>1235</v>
@@ -552,7 +552,7 @@
         <v>3</v>
       </c>
       <c r="F3" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="G3" t="s">
         <v>4</v>

</xml_diff>